<commit_message>
reduced excess code in createMatchFixtures
</commit_message>
<xml_diff>
--- a/static/excel/players_list.xlsx
+++ b/static/excel/players_list.xlsx
@@ -424,7 +424,7 @@
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C400">
-      <formula1>"Aquila,Orion,Cygnus,Pegasus"</formula1>
+      <formula1>"Pegasus,Orion,Aquila,Cygnus"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F400">
       <formula1>"Male,Female"</formula1>
@@ -433,7 +433,7 @@
       <formula1>"Starting,Substitute"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H400">
-      <formula1>"Doubles,Reverse Singles,Singles"</formula1>
+      <formula1>"Singles"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>